<commit_message>
Refinement Class Diagram, Update Stundenliste
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-FlorianHenneke.xlsx
+++ b/stundenlisten/Stundenliste-FlorianHenneke.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michi\OTH\GIT\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tmp\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B322BCF2-D30C-4215-AB48-BA3012ABD39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5099A6F6-EDF2-4709-92DE-B3EA0832CB86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="465" yWindow="45" windowWidth="15165" windowHeight="17430" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>libsigrok integration, WebApp tests, vpn &amp; vnc connection. Wiederkehrende Fehler &amp; VPN/VNC dokumentiert</t>
+  </si>
+  <si>
+    <t>Besprechung</t>
+  </si>
+  <si>
+    <t>Besprechung, erste Design Schritte</t>
+  </si>
+  <si>
+    <t>template_app, Makfiles</t>
+  </si>
+  <si>
+    <t>Design Class Diagram</t>
+  </si>
+  <si>
+    <t>Refinement Class Diagram</t>
   </si>
 </sst>
 </file>
@@ -189,14 +204,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,22 +542,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -651,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C36" si="1">C9+B10</f>
+        <f t="shared" ref="C10:C39" si="1">C9+B10</f>
         <v>15</v>
       </c>
       <c r="D10" t="s">
@@ -876,86 +891,113 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f>C24+B25</f>
         <v>67.5</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
+        <v>44215</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C33" si="2">C25+B26</f>
+        <v>68.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>44217</v>
+      </c>
+      <c r="B27" s="7">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>73.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>44219</v>
+      </c>
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>76.5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>44220</v>
       </c>
-      <c r="B26">
+      <c r="B29">
         <v>9</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>85.5</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>44221</v>
+      </c>
+      <c r="B30" s="7">
+        <v>5</v>
+      </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
+        <f t="shared" si="2"/>
+        <v>90.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>44223</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1.5</v>
+      </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <f t="shared" si="1"/>
-        <v>76.5</v>
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update stundenliste + added signed version of stundenliste
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-FlorianHenneke.xlsx
+++ b/stundenlisten/Stundenliste-FlorianHenneke.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tmp\https_RPOSC\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE594599-2B42-49A6-9498-9E4019C9AD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B537642-C920-4383-8F19-EE4037FB2E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2304" windowWidth="16404" windowHeight="9420" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Studenliste von Florian Henneke</t>
   </si>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C44" si="0">SUM(C7, B8)</f>
+        <f t="shared" ref="C8:C45" si="0">SUM(C7, B8)</f>
         <v>20</v>
       </c>
       <c r="D8" t="s">
@@ -1229,7 +1229,19 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="3"/>
+      <c r="A45" s="3">
+        <v>44461</v>
+      </c>
+      <c r="B45" s="6">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3"/>

</xml_diff>